<commit_message>
修改 [POL Code] 为[Trunk POL]
</commit_message>
<xml_diff>
--- a/ExcelConvertTools2/Config.xlsx
+++ b/ExcelConvertTools2/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Xiong Program\CSharpObject\OtherProgram\ExcelConvertToolsXiongSetup\ExcelConvertToolsXiongSetup\ExcelConvertTools2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F0B2486-4BD7-44A3-9ED6-B2BC706CEECB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4C66696-1A8D-4629-A0FB-0C72E0B589A4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21705" windowHeight="15196" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="64">
   <si>
     <t>Trunk Vessel</t>
   </si>
@@ -242,7 +242,11 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>CNGUA</t>
+    <t>CNNSA</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Y</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1248,8 +1252,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{512016DE-072A-4D66-AFFB-726386210645}">
   <dimension ref="A1:AV2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="X1" workbookViewId="0">
-      <selection activeCell="AK3" sqref="AK3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -1416,7 +1420,9 @@
       <c r="C2" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D2" s="1"/>
+      <c r="D2" s="1" t="s">
+        <v>63</v>
+      </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1" t="s">
         <v>47</v>
@@ -1425,9 +1431,7 @@
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
-      <c r="K2" s="1" t="s">
-        <v>47</v>
-      </c>
+      <c r="K2" s="1"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1" t="s">
         <v>47</v>
@@ -1494,7 +1498,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>

</xml_diff>